<commit_message>
Mudifique as funções, junte as planilhas
</commit_message>
<xml_diff>
--- a/A1 LP.xlsx
+++ b/A1 LP.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acost\OneDrive\Documentos\Fgv\LP\A1 LP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\Estudo\FGV\2º Semestre\Linguagens de Programação\A1.5\Ed-Sheeran-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CAB21C-5D00-4FFE-B5D8-D544D5C8D02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C2C318-1CBF-467A-8BB0-A84DBDBBCE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EdSheeran" sheetId="1" r:id="rId1"/>
+    <sheet name="Albuns" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Albuns!$A$1:$B$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EdSheeran!$A$1:$D$110</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="234">
   <si>
     <t>Música</t>
   </si>
@@ -1608,6 +1610,9 @@
   <si>
     <t>Letra</t>
   </si>
+  <si>
+    <t>Prêmios</t>
+  </si>
 </sst>
 </file>
 
@@ -1616,7 +1621,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1627,6 +1632,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1637,6 +1643,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1670,18 +1690,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1703,7 +1725,6 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1732,10 +1753,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1743,26 +1765,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1776,7 +1778,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
@@ -1844,6 +1846,26 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1858,17 +1880,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E110" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:E110" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
     <sortCondition ref="C1:C110"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Música" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Album" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tempo" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Música" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Album" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tempo" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Popularidade" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Letra" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Letra" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2077,9 +2099,7 @@
   </sheetPr>
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2089,7 +2109,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3976,10 +3996,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3987,4 +4007,106 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBCD12D-57BA-49EE-B11E-C96AFED356B9}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B11" xr:uid="{CEBCD12D-57BA-49EE-B11E-C96AFED356B9}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mudifique as funções, cria a pasta imagem, mude as imagens para pasta imagem
</commit_message>
<xml_diff>
--- a/A1 LP.xlsx
+++ b/A1 LP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\Estudo\FGV\2º Semestre\Linguagens de Programação\A1.5\Ed-Sheeran-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\Estudo\FGV\2º Semestre\Linguagens de Programação\A1.75\Ed-Sheeran-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C2C318-1CBF-467A-8BB0-A84DBDBBCE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4A981-E73E-436C-9AC1-13158A07E491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1621,7 +1621,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1655,14 +1655,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1690,7 +1682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1703,7 +1695,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2109,7 +2100,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">

</xml_diff>